<commit_message>
pull changes from cloud
</commit_message>
<xml_diff>
--- a/core/stream_guild.xlsx
+++ b/core/stream_guild.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="28800" windowHeight="12630" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="609400404223983664" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="609400404223983664_youtube" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1076954067823251617" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1076954067823251617_youtube" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1000585847873220739" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1000585847873220739_youtube" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="987051677045624912" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="987051677045624912_youtube" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="609400404223983664" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="609400404223983664_youtube" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="1076954067823251617" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="1076954067823251617_youtube" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="1000585847873220739" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="1000585847873220739_youtube" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="987051677045624912" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="987051677045624912_youtube" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="144525" fullCalcOnLoad="1"/>
@@ -1098,7 +1098,7 @@
     <row r="1">
       <c r="C1" s="0" t="inlineStr">
         <is>
-          <t>1141074520803921970</t>
+          <t>1135594725156601937</t>
         </is>
       </c>
     </row>
@@ -1186,7 +1186,7 @@
     <row r="1">
       <c r="C1" s="0" t="inlineStr">
         <is>
-          <t>1141074520803921970</t>
+          <t>1135594725156601937</t>
         </is>
       </c>
     </row>
@@ -1223,7 +1223,7 @@
       </c>
       <c r="G2" s="3" t="inlineStr">
         <is>
-          <t>ga2BNK30Pv0,Hh-Gny6H8fw,Sw3HToXF2uc,4-nLzR9GVu0,ZJAs69NY__k,61pCygus9Ok,D7aLMfQwqCY,-jZW07fxQBs,ovkJ7l7dCKI</t>
+          <t>ga2BNK30Pv0,Hh-Gny6H8fw,Sw3HToXF2uc,4-nLzR9GVu0,ZJAs69NY__k,61pCygus9Ok,D7aLMfQwqCY,-jZW07fxQBs,ovkJ7l7dCKI,5ywARf7L35U</t>
         </is>
       </c>
     </row>
@@ -1306,7 +1306,7 @@
       </c>
       <c r="C5" s="0" t="inlineStr">
         <is>
-          <t>None,kLYOmpR-WTs</t>
+          <t>None,kLYOmpR-WTs,YGXF14e3XS4</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -1326,7 +1326,7 @@
       </c>
       <c r="G5" s="3" t="inlineStr">
         <is>
-          <t>mvLCbwzf7Fw,SizDUmbnWNk,XA8SQ49eULc,2fbuxe_K0NI,OJMHrnZUMTE,wjCANhQFs2k,J8dvBe4rGz0,jcynQNgVGlA,T-gfBgxFZX8,GraWAA-5lGA,7tmWUCDgEJk,XU46ItenHuI</t>
+          <t>mvLCbwzf7Fw,SizDUmbnWNk,XA8SQ49eULc,2fbuxe_K0NI,OJMHrnZUMTE,wjCANhQFs2k,J8dvBe4rGz0,jcynQNgVGlA,T-gfBgxFZX8,GraWAA-5lGA,7tmWUCDgEJk,XU46ItenHuI,HEE4gtFvA-E,oCFvnaYW0qI,pHYMlt8j4yA,0Y5fYqlkclI,LMW9zpzQdEw,VSy_q-fi7i0,_TSV8mI0PFw,LXv4w2q3SnI,FKBBJbwQOms,Wza0o6ptS-A,YGXF14e3XS4,LLecLw2kSlQ,QWOMNNR4Z5g,HJMT2vA3WYo,GAAhG5c86RA,lBvNe5YF-yE,sBF0UbN3TxQ</t>
         </is>
       </c>
     </row>
@@ -1552,7 +1552,7 @@
       </c>
       <c r="G2" s="3" t="inlineStr">
         <is>
-          <t>vppYemSrDfk,iQ5u1GMOGc8,5MMWKgVbEgk,3Q2LZ-YJhp0</t>
+          <t>vppYemSrDfk,iQ5u1GMOGc8,5MMWKgVbEgk,3Q2LZ-YJhp0,6n0hbcD0ooU</t>
         </is>
       </c>
     </row>

</xml_diff>